<commit_message>
tambah ringkasan hasil test
</commit_message>
<xml_diff>
--- a/Spesifikasi fitur .xlsx
+++ b/Spesifikasi fitur .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milashania/Desktop/Mila/Work/Mandiri/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milashania/Desktop/Mila/Work/Mandiri/XYZApplication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457CD476-79B1-DF41-B655-773B35C18236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F646C7-02A6-254F-82D4-95EF2357D253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4840" yWindow="500" windowWidth="19260" windowHeight="16940" xr2:uid="{D024CB7F-77A3-C948-9169-8B09EB770BD6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Modul</t>
   </si>
@@ -60,12 +60,6 @@
     <t>Sebagai user, saya dapat login sebagai pengguna menggunakan biometrik</t>
   </si>
   <si>
-    <t xml:space="preserve">Sebagai user, saya dapat melakukan registrasi </t>
-  </si>
-  <si>
-    <t>Sebagai user, saya dapat melihat dan menentukan proses registrasi setelah menentukan syarat dan ketentuan</t>
-  </si>
-  <si>
     <t>Sebagai user, saya dapat melakukan proses verifikasi OTP, sehingga saya dapat melanjutkan proses verfikasi</t>
   </si>
   <si>
@@ -84,15 +78,6 @@
     <t>Sebagai user, saya dapat melihat profile, sehingga saya dapat melihat data diri yang sesuai dengan data registrasi</t>
   </si>
   <si>
-    <t xml:space="preserve">Sebagai user, saya dapat melakukan pengaturan PIN, sehingga saya dapat membuat PIN baru </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sebagai user, saya dapat melihat pengaturan kata sandi, sehingga saya dapat mengubah kata sandi </t>
-  </si>
-  <si>
-    <t>Sebagai user, saya dapat melihat profile, sehingga saya dapat mengubah data registrasi yang telah dibuat</t>
-  </si>
-  <si>
     <t>Pembayaran</t>
   </si>
   <si>
@@ -160,6 +145,57 @@
   </si>
   <si>
     <t xml:space="preserve">Melihat status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebagai user, saya dapat melakukan registrasi dengan mengisi form yang ada </t>
+  </si>
+  <si>
+    <t>Sebagai user, saya dapat membac dan menentukan syarat dan ketentuan yang berlaku di aplikasi</t>
+  </si>
+  <si>
+    <t>Sebagai user, saya dapat melihat profile, sehingga saya dapat mengubah data registrasi yang telah dimasukkan</t>
+  </si>
+  <si>
+    <t>Sebagai user, saya dapat melihat pengaturan kata sandi, sehingga saya dapat mengubah kata sandi pada akun saya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebagai user, saya dapat melakukan pengaturan PIN, sehingga saya dapat membuat PIN baru pada akun saya </t>
+  </si>
+  <si>
+    <t>Sebagai user, saya dapat melihat alert pada kolom yang tidak sesuai pada form peminjaman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebagai user, saya tidak dapat melakukan pengubahan kata sandi apabila kata sandi lama tidak sesuai </t>
+  </si>
+  <si>
+    <t>Sebagai user, saya tidak dapat mengubah kata sandi apabila konfirmasi kata sandi tidak sesuai dengan kata sandi baru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebagai user, saya tidak dapat mengubah kata sandi apabila saya memasukkan kata sandi dengan format yang tidak sesuai </t>
+  </si>
+  <si>
+    <t>Sebagai user, saya tidak dapat melakukan pengubahan PIN apabila PIN lama tidak sesuai</t>
+  </si>
+  <si>
+    <t>Sebagai user, saya tidak dapat mengubah PIN apabila konfirmasi PIN tidak sesuai dengan kata sandi baru</t>
+  </si>
+  <si>
+    <t>Sebagai user, saya dapat melihat alert pada kolom yang tidak sesuai pada form (Contoh: kolom mandatory tidak diisi)</t>
+  </si>
+  <si>
+    <t>Sebagai user, saya dapat melakukan filter berdasarkan riwayat pembayaran</t>
+  </si>
+  <si>
+    <t>Riwayat Peminjaman</t>
+  </si>
+  <si>
+    <t>Melihat Riwayat Menu Peminjaman</t>
+  </si>
+  <si>
+    <t>Sebagai user, saya dapat melakukan filter berdasarkan riwayat peminjaman</t>
+  </si>
+  <si>
+    <t>Sebagai user, saya dapat melihat menu peminjaman sehingga saya dapat melihat riwayat peminjaman</t>
   </si>
 </sst>
 </file>
@@ -203,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -212,13 +248,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,16 +564,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F27EF9F-595B-F84D-9A55-9DBEF940286B}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="51.1640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -560,10 +590,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -571,184 +601,265 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>26</v>
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3" t="s">
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="C30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>24</v>
+    </row>
+    <row r="31" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B17:B18"/>
+  <mergeCells count="17">
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>